<commit_message>
Added logic for inserting data into Vars table
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring1415.xlsx
+++ b/src/main/resources/Spring1415.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
-    <sheet name="BasicData" sheetId="1" r:id="rId1"/>
+    <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="3" r:id="rId2"/>
     <sheet name="CompanyData" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -21,21 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="179">
   <si>
     <t>Item</t>
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Quarter</t>
-  </si>
-  <si>
-    <t>Spring</t>
   </si>
   <si>
     <t>Layout_Section1</t>
@@ -884,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,54 +896,38 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
         <v>10</v>
       </c>
     </row>
@@ -971,298 +946,298 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1280,33 +1255,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1314,16 +1289,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>51</v>
@@ -1331,16 +1306,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>17</v>
@@ -1348,16 +1323,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
         <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1365,16 +1340,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>59</v>
@@ -1382,16 +1357,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E7">
         <v>48</v>
@@ -1399,16 +1374,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>41</v>
@@ -1416,16 +1391,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>35</v>
@@ -1433,16 +1408,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <v>45</v>
@@ -1450,16 +1425,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>55</v>
       </c>
       <c r="E11">
         <v>61</v>
@@ -1467,16 +1442,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E12">
         <v>62</v>
@@ -1484,16 +1459,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E13">
         <v>38</v>
@@ -1501,16 +1476,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14">
         <v>47</v>
@@ -1518,16 +1493,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>16</v>
@@ -1535,16 +1510,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
         <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
       </c>
       <c r="E16">
         <v>49</v>
@@ -1552,16 +1527,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>26</v>
@@ -1569,16 +1544,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E18">
         <v>54</v>
@@ -1586,16 +1561,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>15</v>
@@ -1603,16 +1578,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1620,16 +1595,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E21">
         <v>46</v>
@@ -1637,16 +1612,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E22">
         <v>32</v>
@@ -1654,16 +1629,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -1671,16 +1646,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E24">
         <v>12</v>
@@ -1688,16 +1663,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E25">
         <v>36</v>
@@ -1705,16 +1680,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E26">
         <v>31</v>
@@ -1722,16 +1697,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E27">
         <v>19</v>
@@ -1739,16 +1714,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E28">
         <v>44</v>
@@ -1756,16 +1731,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E29">
         <v>33</v>
@@ -1773,16 +1748,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
         <v>52</v>
-      </c>
-      <c r="D30" t="s">
-        <v>55</v>
       </c>
       <c r="E30">
         <v>18</v>
@@ -1790,16 +1765,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E31">
         <v>28</v>
@@ -1807,16 +1782,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E32">
         <v>9</v>
@@ -1824,16 +1799,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E33">
         <v>6</v>
@@ -1841,16 +1816,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E34">
         <v>21</v>
@@ -1858,16 +1833,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E35">
         <v>29</v>
@@ -1875,16 +1850,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E36">
         <v>67</v>
@@ -1892,16 +1867,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1909,16 +1884,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E38">
         <v>43</v>
@@ -1926,16 +1901,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E39">
         <v>34</v>
@@ -1943,16 +1918,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" t="s">
         <v>52</v>
-      </c>
-      <c r="D40" t="s">
-        <v>55</v>
       </c>
       <c r="E40">
         <v>25</v>
@@ -1960,16 +1935,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E41">
         <v>69</v>
@@ -1977,16 +1952,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E42">
         <v>63</v>
@@ -1994,16 +1969,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -2011,16 +1986,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E44">
         <v>70</v>
@@ -2028,16 +2003,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E45">
         <v>23</v>
@@ -2045,16 +2020,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E46">
         <v>11</v>
@@ -2062,16 +2037,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E47">
         <v>27</v>
@@ -2079,16 +2054,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E48">
         <v>22</v>
@@ -2096,16 +2071,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E49">
         <v>24</v>
@@ -2113,16 +2088,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E50">
         <v>42</v>
@@ -2130,16 +2105,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E51">
         <v>65</v>
@@ -2147,16 +2122,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E52">
         <v>30</v>
@@ -2164,16 +2139,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E53">
         <v>71</v>
@@ -2181,16 +2156,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E54">
         <v>60</v>
@@ -2198,16 +2173,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B55" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E55">
         <v>58</v>
@@ -2215,16 +2190,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D56" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E56">
         <v>10</v>
@@ -2232,16 +2207,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" t="s">
         <v>52</v>
-      </c>
-      <c r="D57" t="s">
-        <v>55</v>
       </c>
       <c r="E57">
         <v>50</v>
@@ -2249,16 +2224,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E58">
         <v>55</v>
@@ -2266,16 +2241,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E59">
         <v>40</v>
@@ -2283,16 +2258,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D60" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E60">
         <v>57</v>
@@ -2300,16 +2275,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E61">
         <v>64</v>
@@ -2317,16 +2292,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E62">
         <v>39</v>
@@ -2334,16 +2309,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C63" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D63" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E63">
         <v>52</v>
@@ -2351,16 +2326,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E64">
         <v>37</v>
@@ -2368,16 +2343,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E65">
         <v>14</v>
@@ -2385,16 +2360,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C66" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E66">
         <v>68</v>
@@ -2402,16 +2377,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E67">
         <v>53</v>
@@ -2419,16 +2394,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E68">
         <v>72</v>
@@ -2436,16 +2411,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E69">
         <v>20</v>
@@ -2453,16 +2428,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B70" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C70" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2470,16 +2445,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D71" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E71">
         <v>13</v>

</xml_diff>

<commit_message>
Added logic to update duplicated values
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring1415.xlsx
+++ b/src/main/resources/Spring1415.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="182">
   <si>
     <t>Item</t>
   </si>
@@ -558,6 +558,15 @@
   </si>
   <si>
     <t>Company Name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Spring</t>
   </si>
 </sst>
 </file>
@@ -875,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,41 +902,57 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>179</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>16</v>
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added logic to parse categories and companies
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring1415.xlsx
+++ b/src/main/resources/Spring1415.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="3" r:id="rId2"/>
-    <sheet name="CompanyData" sheetId="4" r:id="rId3"/>
+    <sheet name="Companies" sheetId="4" r:id="rId3"/>
     <sheet name="TableMappings" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -63,9 +63,6 @@
     <t>Full Time</t>
   </si>
   <si>
-    <t>Work Authorizations</t>
-  </si>
-  <si>
     <t>J-1 Student Visa</t>
   </si>
   <si>
@@ -552,15 +549,6 @@
     <t>Table</t>
   </si>
   <si>
-    <t>Work Authorization Desired</t>
-  </si>
-  <si>
-    <t>Majors Recruited</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -577,6 +565,18 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Work Authorization</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Position Type</t>
   </si>
 </sst>
 </file>
@@ -912,7 +912,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B2">
         <v>2015</v>
@@ -920,10 +920,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -975,304 +975,306 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1284,39 +1286,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s">
-        <v>177</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1324,13 +1335,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -1341,13 +1352,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1358,16 +1369,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1375,16 +1386,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>59</v>
@@ -1392,16 +1403,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7">
         <v>48</v>
@@ -1409,13 +1420,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1426,13 +1437,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1443,13 +1454,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1460,16 +1471,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11">
         <v>61</v>
@@ -1477,16 +1488,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12">
         <v>62</v>
@@ -1494,16 +1505,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13">
         <v>38</v>
@@ -1511,16 +1522,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14">
         <v>47</v>
@@ -1528,13 +1539,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -1545,16 +1556,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16">
         <v>49</v>
@@ -1562,13 +1573,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1579,16 +1590,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18">
         <v>54</v>
@@ -1596,13 +1607,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -1613,13 +1624,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1630,16 +1641,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21">
         <v>46</v>
@@ -1647,16 +1658,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22">
         <v>32</v>
@@ -1664,16 +1675,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -1681,16 +1692,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E24">
         <v>12</v>
@@ -1698,16 +1709,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25">
         <v>36</v>
@@ -1715,16 +1726,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E26">
         <v>31</v>
@@ -1732,16 +1743,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27">
         <v>19</v>
@@ -1749,16 +1760,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28">
         <v>44</v>
@@ -1766,16 +1777,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29">
         <v>33</v>
@@ -1783,16 +1794,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30">
         <v>18</v>
@@ -1800,13 +1811,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -1817,13 +1828,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -1834,16 +1845,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E33">
         <v>6</v>
@@ -1851,16 +1862,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E34">
         <v>21</v>
@@ -1868,13 +1879,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -1885,16 +1896,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36">
         <v>67</v>
@@ -1902,16 +1913,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1919,16 +1930,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E38">
         <v>43</v>
@@ -1936,16 +1947,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E39">
         <v>34</v>
@@ -1953,16 +1964,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E40">
         <v>25</v>
@@ -1970,16 +1981,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E41">
         <v>69</v>
@@ -1987,16 +1998,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E42">
         <v>63</v>
@@ -2004,13 +2015,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -2021,13 +2032,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2038,13 +2049,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -2055,13 +2066,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -2072,16 +2083,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E47">
         <v>27</v>
@@ -2089,13 +2100,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -2106,16 +2117,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49">
         <v>24</v>
@@ -2123,16 +2134,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50">
         <v>42</v>
@@ -2140,13 +2151,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
@@ -2157,16 +2168,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E52">
         <v>30</v>
@@ -2174,16 +2185,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53">
         <v>71</v>
@@ -2191,16 +2202,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E54">
         <v>60</v>
@@ -2208,13 +2219,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -2225,16 +2236,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E56">
         <v>10</v>
@@ -2242,16 +2253,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E57">
         <v>50</v>
@@ -2259,13 +2270,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -2276,13 +2287,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
@@ -2293,16 +2304,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E60">
         <v>57</v>
@@ -2310,13 +2321,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
@@ -2327,13 +2338,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -2344,16 +2355,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E63">
         <v>52</v>
@@ -2361,16 +2372,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E64">
         <v>37</v>
@@ -2378,16 +2389,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E65">
         <v>14</v>
@@ -2395,13 +2406,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
@@ -2412,16 +2423,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E67">
         <v>53</v>
@@ -2429,13 +2440,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D68" t="s">
         <v>9</v>
@@ -2446,13 +2457,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
@@ -2463,16 +2474,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2480,16 +2491,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C71" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E71">
         <v>13</v>
@@ -2504,21 +2515,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>